<commit_message>
feat:field validators server side
</commit_message>
<xml_diff>
--- a/template/template-v2.xlsx
+++ b/template/template-v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Ifinworth\ifinworth\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54DCAD5-0227-4C14-870A-88FB63B17EAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B09F0A-F2DD-4165-9439-5D7DE300417E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{B1689DFF-EE47-4FC0-B162-7D2AF1E3E42F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="2" xr2:uid="{B1689DFF-EE47-4FC0-B162-7D2AF1E3E42F}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;L" sheetId="2" r:id="rId1"/>
@@ -1541,7 +1541,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D177"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -3141,8 +3141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFC96DA0-E1F5-4262-81B7-A5E910BCEBDB}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8984375" defaultRowHeight="13.8"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="C26" s="45"/>
       <c r="D26" s="45">
-        <f>-((BS!D6+BS!D7+BS!D8+BS!D9+BS!D10+BS!D13+BS!D14+BS!D15+ BS!D16)+'P&amp;L'!E32-(BS!B6+BS!B7+BS!B8+BS!B9+BS!B10+BS!B13+BS!B14+BS!B15))</f>
+        <f>-((BS!D6+BS!D7+BS!D8+BS!D9+BS!D10+BS!D13+BS!D14+BS!D15+ BS!D16)+'P&amp;L'!E32-(BS!B6+BS!B7+BS!B8+BS!B9+BS!B10+BS!B13+BS!B14+BS!B15+BS!D16))</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>